<commit_message>
updated tools information in Sheet1
</commit_message>
<xml_diff>
--- a/Topics.xlsx
+++ b/Topics.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="204">
   <si>
     <t>Installation</t>
   </si>
@@ -534,10 +535,121 @@
     <t>Agile Basics</t>
   </si>
   <si>
-    <t xml:space="preserve">                   Spring Live Project</t>
-  </si>
-  <si>
     <t>Angular Project</t>
+  </si>
+  <si>
+    <t>AWS Basics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Spring Deep Dive</t>
+  </si>
+  <si>
+    <t>DEMO URL</t>
+  </si>
+  <si>
+    <t>Video URL</t>
+  </si>
+  <si>
+    <t>Java Basics &amp; Java 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Testing </t>
+  </si>
+  <si>
+    <t>IDE Basics</t>
+  </si>
+  <si>
+    <t>Build tools and Maven</t>
+  </si>
+  <si>
+    <t>GIT-SCM</t>
+  </si>
+  <si>
+    <t>https://git-scm.com/downloads</t>
+  </si>
+  <si>
+    <t>Tortoise git</t>
+  </si>
+  <si>
+    <t>https://tortoisegit.org/</t>
+  </si>
+  <si>
+    <t>http://mirrors.estointernet.in/apache/maven/maven-3/3.6.0/binaries/apache-maven-3.6.0-bin.zip</t>
+  </si>
+  <si>
+    <t>STS</t>
+  </si>
+  <si>
+    <t>https://spring.io/tools</t>
+  </si>
+  <si>
+    <t>https://www.oracle.com/technetwork/database/database-technologies/express-edition/downloads/index.html</t>
+  </si>
+  <si>
+    <t>Register and Download</t>
+  </si>
+  <si>
+    <t>https://www.getpostman.com/downloads/</t>
+  </si>
+  <si>
+    <t>No Chrome plugin</t>
+  </si>
+  <si>
+    <t>Postman</t>
+  </si>
+  <si>
+    <t>VSCode</t>
+  </si>
+  <si>
+    <t>https://code.visualstudio.com/download</t>
+  </si>
+  <si>
+    <t>NodeJs</t>
+  </si>
+  <si>
+    <t>https://nodejs.org/en/download/</t>
+  </si>
+  <si>
+    <t>https://www.oracle.com/technetwork/developer-tools/sql-developer/downloads/index.html</t>
+  </si>
+  <si>
+    <t>https://jenkins.io/download/</t>
+  </si>
+  <si>
+    <t>Tomcat 8</t>
+  </si>
+  <si>
+    <t>https://tomcat.apache.org/download-80.cgi</t>
+  </si>
+  <si>
+    <t>JDK(Java 8)</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Middleware Server</t>
+  </si>
+  <si>
+    <t>CI-CD</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>REST</t>
+  </si>
+  <si>
+    <t>Java IDE</t>
+  </si>
+  <si>
+    <t>Download as WAR</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>Create account for yourself</t>
   </si>
 </sst>
 </file>
@@ -590,7 +702,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -613,11 +725,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -642,18 +774,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,7 +1074,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -934,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -945,9 +1093,11 @@
     <col min="1" max="1" width="38.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>50</v>
@@ -955,376 +1105,382 @@
       <c r="C1" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
       <c r="C4" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
       <c r="C5" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
       <c r="C6" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
       <c r="B14" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
       <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="10"/>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
+      <c r="A18" s="10"/>
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
+      <c r="A19" s="10"/>
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
+      <c r="A20" s="10"/>
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
+      <c r="A21" s="10"/>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
+      <c r="A23" s="10"/>
       <c r="C23" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
+      <c r="A24" s="10"/>
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
+      <c r="A25" s="10"/>
       <c r="C25" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
+      <c r="A26" s="10"/>
       <c r="C26" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
+      <c r="A27" s="10"/>
       <c r="C27" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
+      <c r="A28" s="10"/>
       <c r="C28" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
+      <c r="A29" s="10"/>
       <c r="C29" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
-        <v>23</v>
+      <c r="A31" s="10" t="s">
+        <v>173</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
+      <c r="A32" s="10"/>
       <c r="C32" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="12"/>
+      <c r="A33" s="10"/>
       <c r="C33" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
+      <c r="A34" s="10"/>
       <c r="C34" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
+      <c r="A35" s="10"/>
       <c r="C35" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
+      <c r="A37" s="10"/>
       <c r="C37" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
+      <c r="A38" s="10"/>
       <c r="C38" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
+      <c r="A39" s="10"/>
       <c r="C39" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
+      <c r="A40" s="10"/>
       <c r="C40" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
+      <c r="A41" s="10"/>
       <c r="C41" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
+      <c r="A42" s="10"/>
       <c r="C42" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
+      <c r="A44" s="10"/>
       <c r="C44" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
+      <c r="A45" s="10"/>
       <c r="C45" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="12"/>
+      <c r="A46" s="10"/>
       <c r="C46" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
+      <c r="A47" s="10"/>
       <c r="C47" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="12"/>
+      <c r="A48" s="10"/>
       <c r="C48" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="12"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="12"/>
+      <c r="A50" s="10"/>
       <c r="C50" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="12"/>
+      <c r="A51" s="10"/>
       <c r="C51" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="12"/>
+      <c r="A52" s="10"/>
       <c r="C52" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="12"/>
+      <c r="A53" s="10"/>
       <c r="C53" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="12"/>
+      <c r="A54" s="10"/>
       <c r="C54" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="12"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="12"/>
+      <c r="A56" s="10"/>
       <c r="C56" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="12"/>
+      <c r="A57" s="10"/>
       <c r="C57" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="12"/>
+      <c r="A58" s="10"/>
       <c r="C58" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="12"/>
+      <c r="A59" s="10"/>
       <c r="C59" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="12"/>
+      <c r="A60" s="10"/>
       <c r="C60" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="7"/>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C61" s="10"/>
+      <c r="C61" s="13"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1332,98 +1488,98 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="12"/>
+      <c r="A63" s="10"/>
       <c r="C63" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="12"/>
+      <c r="A64" s="10"/>
       <c r="C64" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="12"/>
+      <c r="A65" s="10"/>
       <c r="C65" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="12"/>
+      <c r="A66" s="10"/>
       <c r="C66" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="12"/>
+      <c r="A67" s="10"/>
       <c r="C67" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="12"/>
+      <c r="A68" s="10"/>
       <c r="B68" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="12"/>
+      <c r="A69" s="10"/>
       <c r="C69" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="12"/>
+      <c r="A70" s="10"/>
       <c r="C70" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="12"/>
+      <c r="A71" s="10"/>
       <c r="C71" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="12"/>
+      <c r="A72" s="10"/>
       <c r="B72" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="12"/>
+      <c r="A73" s="10"/>
       <c r="C73" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="12"/>
+      <c r="A74" s="10"/>
       <c r="C74" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="12"/>
+      <c r="A75" s="10"/>
       <c r="C75" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="12"/>
+      <c r="A76" s="10"/>
       <c r="C76" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="7"/>
-      <c r="B77" s="10" t="s">
+      <c r="B77" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C77" s="10"/>
+      <c r="C77" s="13"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="12" t="s">
+      <c r="A78" s="10" t="s">
         <v>162</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -1431,145 +1587,145 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="12"/>
+      <c r="A79" s="10"/>
       <c r="C79" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="12"/>
+      <c r="A80" s="10"/>
       <c r="C80" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="12"/>
+      <c r="A81" s="10"/>
       <c r="C81" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="12"/>
+      <c r="A82" s="10"/>
       <c r="C82" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="12"/>
+      <c r="A83" s="10"/>
       <c r="B83" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="12"/>
+      <c r="A84" s="10"/>
       <c r="C84" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="12"/>
+      <c r="A85" s="10"/>
       <c r="C85" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="12"/>
+      <c r="A86" s="10"/>
       <c r="C86" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="7"/>
-      <c r="B87" s="10" t="s">
+      <c r="B87" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C87" s="10"/>
+      <c r="C87" s="13"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="12" t="s">
-        <v>77</v>
+      <c r="A88" s="10" t="s">
+        <v>170</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="12"/>
+      <c r="A89" s="10"/>
       <c r="C89" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="12"/>
+      <c r="A90" s="10"/>
       <c r="B90" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="12"/>
+      <c r="A91" s="10"/>
       <c r="C91" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="12"/>
+      <c r="A92" s="10"/>
       <c r="C92" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="12"/>
+      <c r="A93" s="10"/>
       <c r="C93" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="12"/>
+      <c r="A94" s="10"/>
       <c r="B94" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C94" s="6"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="12"/>
+      <c r="A95" s="10"/>
       <c r="C95" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="12"/>
+      <c r="A96" s="10"/>
       <c r="C96" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="12"/>
+      <c r="A97" s="10"/>
       <c r="B97" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="12"/>
+      <c r="A98" s="10"/>
       <c r="C98" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="12"/>
+      <c r="A99" s="10"/>
       <c r="C99" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="7"/>
-      <c r="B100" s="10" t="s">
+      <c r="B100" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C100" s="10"/>
+      <c r="C100" s="13"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -1577,44 +1733,44 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="12"/>
+      <c r="A102" s="10"/>
       <c r="C102" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="12"/>
+      <c r="A103" s="10"/>
       <c r="C103" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="12"/>
+      <c r="A104" s="10"/>
       <c r="C104" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="12"/>
+      <c r="A105" s="10"/>
       <c r="C105" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="12"/>
+      <c r="A106" s="10"/>
       <c r="C106" s="2" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="7"/>
-      <c r="B107" s="10" t="s">
+      <c r="B107" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C107" s="10"/>
+      <c r="C107" s="13"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="12" t="s">
+      <c r="A108" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -1623,57 +1779,57 @@
       <c r="C108" s="3"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="12"/>
+      <c r="A109" s="10"/>
       <c r="C109" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="12"/>
+      <c r="A110" s="10"/>
       <c r="C110" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="12"/>
+      <c r="A111" s="10"/>
       <c r="C111" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="12"/>
+      <c r="A112" s="10"/>
       <c r="B112" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C112" s="6"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="12"/>
+      <c r="A113" s="10"/>
       <c r="C113" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="12"/>
+      <c r="A114" s="10"/>
       <c r="C114" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="12"/>
+      <c r="A115" s="10"/>
       <c r="C115" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="7"/>
-      <c r="B116" s="10" t="s">
+      <c r="B116" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C116" s="10"/>
+      <c r="C116" s="13"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="12" t="s">
+      <c r="A117" s="10" t="s">
         <v>163</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -1684,71 +1840,71 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="12"/>
+      <c r="A118" s="10"/>
       <c r="C118" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="12"/>
+      <c r="A119" s="10"/>
       <c r="C119" s="6" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="12"/>
+      <c r="A120" s="10"/>
       <c r="C120" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="12"/>
+      <c r="A121" s="10"/>
       <c r="C121" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="12"/>
+      <c r="A122" s="10"/>
       <c r="C122" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="12"/>
+      <c r="A123" s="10"/>
       <c r="C123" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="12"/>
+      <c r="A124" s="10"/>
       <c r="C124" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="12"/>
+      <c r="A125" s="10"/>
       <c r="C125" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="12"/>
+      <c r="A126" s="10"/>
       <c r="C126" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="12"/>
+      <c r="A127" s="10"/>
       <c r="C127" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="7"/>
-      <c r="B128" s="10" t="s">
+      <c r="B128" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="C128" s="10"/>
+      <c r="C128" s="13"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="11" t="s">
@@ -1772,253 +1928,265 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="7"/>
-      <c r="B132" s="10" t="s">
+      <c r="B132" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C132" s="10"/>
+      <c r="C132" s="13"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="13" t="s">
-        <v>165</v>
+      <c r="A133" s="12" t="s">
+        <v>167</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="13"/>
+      <c r="A134" s="12"/>
       <c r="C134" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="13"/>
+      <c r="A135" s="12"/>
       <c r="C135" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" s="13"/>
-      <c r="B136" s="10" t="s">
+      <c r="A136" s="12"/>
+      <c r="B136" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C136" s="10"/>
+      <c r="C136" s="13"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="13"/>
+      <c r="A137" s="12"/>
       <c r="C137" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" s="13"/>
+      <c r="A138" s="12"/>
       <c r="C138" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" s="13"/>
-      <c r="B139" s="10" t="s">
+      <c r="A139" s="12"/>
+      <c r="B139" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C139" s="10"/>
+      <c r="C139" s="13"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="13"/>
+      <c r="A140" s="12"/>
       <c r="C140" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="13"/>
+      <c r="A141" s="12"/>
       <c r="C141" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="13"/>
+      <c r="A142" s="12"/>
       <c r="C142" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="13"/>
+      <c r="A143" s="12"/>
       <c r="C143" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="13"/>
-      <c r="B144" s="10" t="s">
+      <c r="A144" s="12"/>
+      <c r="B144" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C144" s="10"/>
+      <c r="C144" s="13"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" s="13"/>
+      <c r="A145" s="12"/>
       <c r="C145" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="13"/>
+      <c r="A146" s="12"/>
       <c r="C146" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="13"/>
+      <c r="A147" s="12"/>
       <c r="C147" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" s="13"/>
-      <c r="B148" s="10" t="s">
+      <c r="A148" s="12"/>
+      <c r="B148" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C148" s="10"/>
+      <c r="C148" s="13"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="13"/>
+      <c r="A149" s="12"/>
       <c r="C149" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="13"/>
+      <c r="A150" s="12"/>
       <c r="C150" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="13"/>
+      <c r="A151" s="12"/>
       <c r="C151" s="5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="13"/>
+      <c r="A152" s="12"/>
       <c r="C152" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="13"/>
+      <c r="A153" s="12"/>
       <c r="C153" s="5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="13"/>
+      <c r="A154" s="12"/>
       <c r="C154" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" s="13"/>
+      <c r="A155" s="12"/>
       <c r="C155" s="5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" s="13"/>
+      <c r="A156" s="12"/>
       <c r="C156" s="5" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" s="13"/>
+      <c r="A157" s="12"/>
       <c r="C157" s="5" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" s="13"/>
+      <c r="A158" s="12"/>
       <c r="C158" s="5" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" s="13"/>
-      <c r="B159" s="10" t="s">
+      <c r="A159" s="12"/>
+      <c r="B159" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C159" s="10"/>
+      <c r="C159" s="13"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" s="13"/>
+      <c r="A160" s="12"/>
       <c r="C160" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" s="13"/>
-      <c r="B161" s="10" t="s">
+      <c r="A161" s="12"/>
+      <c r="B161" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C161" s="10"/>
+      <c r="C161" s="13"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" s="13"/>
+      <c r="A162" s="12"/>
       <c r="C162" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="13"/>
+      <c r="A163" s="12"/>
       <c r="C163" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" s="13"/>
+      <c r="A164" s="12"/>
       <c r="C164" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" s="13"/>
+      <c r="A165" s="12"/>
       <c r="C165" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" s="13"/>
-      <c r="B166" s="10" t="s">
+      <c r="A166" s="12"/>
+      <c r="B166" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C166" s="10"/>
+      <c r="C166" s="13"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" s="13"/>
+      <c r="A167" s="12"/>
       <c r="C167" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" s="13"/>
+      <c r="A168" s="12"/>
       <c r="C168" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" s="1" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A101:A106"/>
-    <mergeCell ref="A108:A115"/>
-    <mergeCell ref="A117:A127"/>
-    <mergeCell ref="A129:A131"/>
-    <mergeCell ref="A133:A168"/>
-    <mergeCell ref="A3:A29"/>
-    <mergeCell ref="A31:A60"/>
-    <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A78:A86"/>
-    <mergeCell ref="A88:A99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B87:C87"/>
     <mergeCell ref="B148:C148"/>
     <mergeCell ref="B159:C159"/>
     <mergeCell ref="B161:C161"/>
@@ -2029,15 +2197,182 @@
     <mergeCell ref="B139:C139"/>
     <mergeCell ref="B144:C144"/>
     <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="A3:A29"/>
+    <mergeCell ref="A31:A60"/>
+    <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A78:A86"/>
+    <mergeCell ref="A88:A99"/>
+    <mergeCell ref="A101:A106"/>
+    <mergeCell ref="A108:A115"/>
+    <mergeCell ref="A117:A127"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="A133:A168"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" customWidth="1"/>
+    <col min="3" max="3" width="88.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="17"/>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Trainer Name. Reduced Course content to one month
</commit_message>
<xml_diff>
--- a/Topics.xlsx
+++ b/Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Narasimha\Interview\Training\trainings\trainings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codebase\trainings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EA517D-03A5-4ECF-A1BE-E97F6C4D78DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D45F30-2024-4B31-B400-AE9C9165462C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="to be deleted" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Softwares" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="308">
   <si>
     <t>Installation</t>
   </si>
@@ -742,24 +742,12 @@
     <t>https://www.mysql.com/downloads/</t>
   </si>
   <si>
-    <t xml:space="preserve">  JPA</t>
-  </si>
-  <si>
     <t xml:space="preserve">  REST</t>
   </si>
   <si>
-    <t xml:space="preserve">  JMS</t>
-  </si>
-  <si>
     <t xml:space="preserve">  MongoDB</t>
   </si>
   <si>
-    <t xml:space="preserve">  Actuator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Security</t>
-  </si>
-  <si>
     <t>Course</t>
   </si>
   <si>
@@ -785,9 +773,6 @@
   </si>
   <si>
     <t>Angular Project</t>
-  </si>
-  <si>
-    <t>AWS Basics</t>
   </si>
   <si>
     <t xml:space="preserve">Unit Testing </t>
@@ -988,6 +973,33 @@
   </si>
   <si>
     <t>SCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  JPA with Hibernate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  JMS/Active MQ/Kafka</t>
+  </si>
+  <si>
+    <t>Total Sessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Security/Oauth/JWT</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Trainer</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>Vamshi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Actuator </t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1193,48 +1205,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1243,53 +1213,96 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1573,7 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A100" sqref="A100:A111"/>
     </sheetView>
   </sheetViews>
@@ -1600,7 +1613,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="28" t="s">
         <v>188</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1613,7 +1626,7 @@
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
         <v>189</v>
@@ -1622,7 +1635,7 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>225</v>
@@ -1632,361 +1645,361 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="37"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>259</v>
+      <c r="A6" s="38" t="s">
+        <v>254</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
+      <c r="A7" s="38"/>
       <c r="C7" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="38"/>
       <c r="C8" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="38"/>
       <c r="C9" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
+      <c r="A11" s="38"/>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
+      <c r="A12" s="38"/>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
+      <c r="A13" s="38"/>
       <c r="C13" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="38"/>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="38"/>
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
+      <c r="A16" s="38"/>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
+      <c r="A17" s="38"/>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
+      <c r="A19" s="38"/>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="38"/>
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
+      <c r="A21" s="38"/>
       <c r="C21" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
+      <c r="A22" s="38"/>
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
+      <c r="A23" s="38"/>
       <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
+      <c r="A24" s="38"/>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
+      <c r="A26" s="38"/>
       <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="19"/>
+      <c r="A27" s="38"/>
       <c r="C27" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
+      <c r="A28" s="38"/>
       <c r="C28" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
+      <c r="A29" s="38"/>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
+      <c r="A30" s="38"/>
       <c r="C30" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="19"/>
+      <c r="A31" s="38"/>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="37"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
-        <v>260</v>
+      <c r="A33" s="38" t="s">
+        <v>255</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="19"/>
+      <c r="A34" s="38"/>
       <c r="C34" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
+      <c r="A35" s="38"/>
       <c r="C35" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="19"/>
+      <c r="A36" s="38"/>
       <c r="C36" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
-      <c r="B37" s="34" t="s">
-        <v>261</v>
+      <c r="A37" s="38"/>
+      <c r="B37" s="20" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="19"/>
+      <c r="A38" s="38"/>
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="19"/>
+      <c r="A39" s="38"/>
       <c r="C39" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
+      <c r="A40" s="38"/>
       <c r="C40" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
+      <c r="A41" s="38"/>
       <c r="C41" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
+      <c r="A42" s="38"/>
       <c r="C42" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
+      <c r="A43" s="38"/>
       <c r="C43" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
+      <c r="A44" s="38"/>
       <c r="B44" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
+      <c r="A45" s="38"/>
       <c r="C45" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
+      <c r="A46" s="38"/>
       <c r="C46" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
+      <c r="A47" s="38"/>
       <c r="C47" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
+      <c r="A48" s="38"/>
       <c r="C48" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="19"/>
+      <c r="A49" s="38"/>
       <c r="C49" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="19"/>
+      <c r="A50" s="38"/>
       <c r="B50" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="19"/>
+      <c r="A51" s="38"/>
       <c r="C51" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
+      <c r="A52" s="38"/>
       <c r="C52" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="19"/>
+      <c r="A53" s="38"/>
       <c r="C53" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="19"/>
+      <c r="A54" s="38"/>
       <c r="C54" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="19"/>
+      <c r="A55" s="38"/>
       <c r="C55" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="19"/>
+      <c r="A56" s="38"/>
       <c r="B56" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="19"/>
+      <c r="A57" s="38"/>
       <c r="C57" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="19"/>
+      <c r="A58" s="38"/>
       <c r="C58" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="19"/>
+      <c r="A59" s="38"/>
       <c r="C59" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="19"/>
+      <c r="A60" s="38"/>
       <c r="C60" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="19"/>
+      <c r="A61" s="38"/>
       <c r="C61" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="21"/>
+      <c r="C62" s="37"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="38" t="s">
         <v>226</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1994,95 +2007,95 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="19"/>
+      <c r="A64" s="38"/>
       <c r="C64" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="19"/>
+      <c r="A65" s="38"/>
       <c r="C65" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="19"/>
+      <c r="A66" s="38"/>
       <c r="C66" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="19"/>
+      <c r="A67" s="38"/>
       <c r="B67" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="19"/>
+      <c r="A68" s="38"/>
       <c r="B68" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="19"/>
+      <c r="A69" s="38"/>
       <c r="C69" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="19"/>
+      <c r="A70" s="38"/>
       <c r="C70" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="19"/>
+      <c r="A71" s="38"/>
       <c r="C71" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="19"/>
+      <c r="A72" s="38"/>
       <c r="B72" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="19"/>
+      <c r="A73" s="38"/>
       <c r="C73" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="19"/>
+      <c r="A74" s="38"/>
       <c r="C74" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="19"/>
+      <c r="A75" s="38"/>
       <c r="C75" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
+      <c r="A76" s="38"/>
       <c r="C76" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C77" s="21"/>
+      <c r="C77" s="37"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="38" t="s">
         <v>227</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -2090,89 +2103,89 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="19"/>
+      <c r="A79" s="38"/>
       <c r="C79" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="19"/>
+      <c r="A80" s="38"/>
       <c r="C80" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="19"/>
+      <c r="A81" s="38"/>
       <c r="C81" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="19"/>
+      <c r="A82" s="38"/>
       <c r="C82" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="19"/>
+      <c r="A83" s="38"/>
       <c r="B83" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="19"/>
+      <c r="A84" s="38"/>
       <c r="C84" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="19"/>
+      <c r="A85" s="38"/>
       <c r="C85" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="19"/>
+      <c r="A86" s="38"/>
       <c r="C86" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
-      <c r="B87" s="21" t="s">
+      <c r="B87" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C87" s="21"/>
+      <c r="C87" s="37"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="19" t="s">
-        <v>265</v>
+      <c r="A88" s="38" t="s">
+        <v>260</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="19"/>
+      <c r="A89" s="38"/>
       <c r="C89" s="2" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="19"/>
+      <c r="A90" s="38"/>
       <c r="C90" s="17" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="19"/>
+      <c r="A91" s="38"/>
       <c r="B91" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C91" s="2"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="19"/>
+      <c r="A92" s="38"/>
       <c r="C92" s="2" t="s">
         <v>71</v>
       </c>
@@ -2181,19 +2194,19 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="19"/>
+      <c r="A93" s="38"/>
       <c r="C93" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="19"/>
+      <c r="A94" s="38"/>
       <c r="C94" s="1" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="19"/>
+      <c r="A95" s="38"/>
       <c r="B95" s="1" t="s">
         <v>169</v>
       </c>
@@ -2202,33 +2215,33 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="19"/>
+      <c r="A96" s="38"/>
       <c r="B96" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C96" s="2"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="19"/>
+      <c r="A97" s="38"/>
       <c r="C97" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="19"/>
+      <c r="A98" s="38"/>
       <c r="C98" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="C99" s="21"/>
+      <c r="C99" s="37"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="19" t="s">
+      <c r="A100" s="38" t="s">
         <v>228</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -2237,44 +2250,44 @@
       <c r="C100" s="2"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="19"/>
+      <c r="A101" s="38"/>
       <c r="C101" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="19"/>
+      <c r="A102" s="38"/>
       <c r="C102" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="19"/>
+      <c r="A103" s="38"/>
       <c r="C103" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="19"/>
+      <c r="A104" s="38"/>
       <c r="B104" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="19"/>
+      <c r="A105" s="38"/>
       <c r="C105" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="19"/>
+      <c r="A106" s="38"/>
       <c r="C106" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="19"/>
+      <c r="A107" s="38"/>
       <c r="B107" s="1" t="s">
         <v>172</v>
       </c>
@@ -2283,38 +2296,38 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="19"/>
+      <c r="A108" s="38"/>
       <c r="C108" s="2" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="19"/>
+      <c r="A109" s="38"/>
       <c r="C109" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="19"/>
+      <c r="A110" s="38"/>
       <c r="C110" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="19"/>
+      <c r="A111" s="38"/>
       <c r="C111" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
-      <c r="B112" s="21" t="s">
+      <c r="B112" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C112" s="21"/>
+      <c r="C112" s="37"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="19" t="s">
+      <c r="A113" s="38" t="s">
         <v>229</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -2325,74 +2338,74 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="19"/>
+      <c r="A114" s="38"/>
       <c r="C114" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="19"/>
+      <c r="A115" s="38"/>
       <c r="C115" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="19"/>
+      <c r="A116" s="38"/>
       <c r="C116" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="19"/>
+      <c r="A117" s="38"/>
       <c r="C117" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="19"/>
+      <c r="A118" s="38"/>
       <c r="C118" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="19"/>
+      <c r="A119" s="38"/>
       <c r="C119" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="19"/>
+      <c r="A120" s="38"/>
       <c r="C120" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="19"/>
+      <c r="A121" s="38"/>
       <c r="C121" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="19"/>
+      <c r="A122" s="38"/>
       <c r="C122" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="19"/>
+      <c r="A123" s="38"/>
       <c r="C123" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
-      <c r="B129" s="21" t="s">
+      <c r="B129" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C129" s="21"/>
+      <c r="C129" s="37"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="20" t="s">
+      <c r="A130" s="39" t="s">
         <v>230</v>
       </c>
       <c r="C130" s="2" t="s">
@@ -2400,224 +2413,224 @@
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="20"/>
+      <c r="A131" s="39"/>
       <c r="C131" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="20"/>
+      <c r="A132" s="39"/>
       <c r="C132" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="20"/>
-      <c r="B133" s="21" t="s">
+      <c r="A133" s="39"/>
+      <c r="B133" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C133" s="21"/>
+      <c r="C133" s="37"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="20"/>
+      <c r="A134" s="39"/>
       <c r="C134" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="20"/>
+      <c r="A135" s="39"/>
       <c r="C135" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" s="20"/>
-      <c r="B136" s="21" t="s">
+      <c r="A136" s="39"/>
+      <c r="B136" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C136" s="21"/>
+      <c r="C136" s="37"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="20"/>
+      <c r="A137" s="39"/>
       <c r="C137" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="20"/>
+      <c r="A138" s="39"/>
       <c r="C138" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="20"/>
+      <c r="A139" s="39"/>
       <c r="C139" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="20"/>
+      <c r="A140" s="39"/>
       <c r="C140" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="20"/>
-      <c r="B141" s="21" t="s">
+      <c r="A141" s="39"/>
+      <c r="B141" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C141" s="21"/>
+      <c r="C141" s="37"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" s="20"/>
+      <c r="A142" s="39"/>
       <c r="C142" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="20"/>
+      <c r="A143" s="39"/>
       <c r="C143" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" s="20"/>
+      <c r="A144" s="39"/>
       <c r="C144" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="20"/>
-      <c r="B145" s="21" t="s">
+      <c r="A145" s="39"/>
+      <c r="B145" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="C145" s="21"/>
+      <c r="C145" s="37"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="20"/>
+      <c r="A146" s="39"/>
       <c r="C146" s="6" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="20"/>
+      <c r="A147" s="39"/>
       <c r="C147" s="4" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="20"/>
+      <c r="A148" s="39"/>
       <c r="C148" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="20"/>
+      <c r="A149" s="39"/>
       <c r="C149" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="20"/>
+      <c r="A150" s="39"/>
       <c r="C150" s="4" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="20"/>
+      <c r="A151" s="39"/>
       <c r="C151" s="4" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="20"/>
+      <c r="A152" s="39"/>
       <c r="C152" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="20"/>
+      <c r="A153" s="39"/>
       <c r="C153" s="4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="20"/>
+      <c r="A154" s="39"/>
       <c r="C154" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="20"/>
+      <c r="A155" s="39"/>
       <c r="C155" s="4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="20"/>
-      <c r="B156" s="21" t="s">
+      <c r="A156" s="39"/>
+      <c r="B156" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="C156" s="21"/>
+      <c r="C156" s="37"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="20"/>
+      <c r="A157" s="39"/>
       <c r="C157" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="20"/>
-      <c r="B158" s="21" t="s">
+      <c r="A158" s="39"/>
+      <c r="B158" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="C158" s="21"/>
+      <c r="C158" s="37"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="20"/>
+      <c r="A159" s="39"/>
       <c r="C159" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="20"/>
+      <c r="A160" s="39"/>
       <c r="C160" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="20"/>
+      <c r="A161" s="39"/>
       <c r="C161" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="20"/>
+      <c r="A162" s="39"/>
       <c r="C162" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="20"/>
-      <c r="B163" s="21" t="s">
+      <c r="A163" s="39"/>
+      <c r="B163" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="C163" s="21"/>
+      <c r="C163" s="37"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="20"/>
+      <c r="A164" s="39"/>
       <c r="C164" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="20"/>
+      <c r="A165" s="39"/>
       <c r="C165" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="25" t="s">
+      <c r="A166" s="31" t="s">
         <v>231</v>
       </c>
       <c r="B166" s="13"/>
@@ -2626,100 +2639,100 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="26"/>
+      <c r="A167" s="32"/>
       <c r="C167" s="1" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" s="26"/>
+      <c r="A168" s="32"/>
       <c r="C168" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" s="26"/>
+      <c r="A169" s="32"/>
       <c r="C169" s="1" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" s="26"/>
+      <c r="A170" s="32"/>
       <c r="C170" s="1" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" s="26"/>
+      <c r="A171" s="32"/>
       <c r="C171" s="1" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" s="26"/>
+      <c r="A172" s="32"/>
       <c r="C172" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173" s="26"/>
+      <c r="A173" s="32"/>
       <c r="C173" s="1" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" s="26"/>
+      <c r="A174" s="32"/>
       <c r="C174" s="1" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="26"/>
+      <c r="A175" s="32"/>
       <c r="C175" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" s="26"/>
+      <c r="A176" s="32"/>
       <c r="C176" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" s="26"/>
+      <c r="A177" s="32"/>
       <c r="C177" s="1" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178" s="26"/>
+      <c r="A178" s="32"/>
       <c r="C178" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="26"/>
+      <c r="A179" s="32"/>
       <c r="C179" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" s="26"/>
+      <c r="A180" s="32"/>
       <c r="C180" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" s="26"/>
+      <c r="A181" s="32"/>
       <c r="C181" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" s="27"/>
+      <c r="A182" s="33"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" s="25" t="s">
+      <c r="A183" s="31" t="s">
         <v>232</v>
       </c>
       <c r="C183" s="1" t="s">
@@ -2727,52 +2740,52 @@
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184" s="26"/>
+      <c r="A184" s="32"/>
       <c r="C184" s="1" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" s="26"/>
+      <c r="A185" s="32"/>
       <c r="C185" s="1" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="26"/>
+      <c r="A186" s="32"/>
       <c r="C186" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="26"/>
+      <c r="A187" s="32"/>
       <c r="C187" s="1" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" s="26"/>
+      <c r="A188" s="32"/>
       <c r="C188" s="1" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" s="26"/>
+      <c r="A189" s="32"/>
       <c r="C189" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190" s="26"/>
+      <c r="A190" s="32"/>
       <c r="C190" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" s="27"/>
+      <c r="A191" s="33"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" s="28" t="s">
+      <c r="A192" s="34" t="s">
         <v>233</v>
       </c>
       <c r="C192" s="1" t="s">
@@ -2780,43 +2793,54 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="29"/>
+      <c r="A193" s="35"/>
       <c r="C193" s="1" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="29"/>
+      <c r="A194" s="35"/>
       <c r="C194" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="29"/>
+      <c r="A195" s="35"/>
       <c r="C195" s="1" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="29"/>
+      <c r="A196" s="35"/>
       <c r="C196" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="29"/>
+      <c r="A197" s="35"/>
       <c r="C197" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" s="30"/>
+      <c r="A198" s="36"/>
       <c r="C198" s="1" t="s">
         <v>217</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="A6:A31"/>
+    <mergeCell ref="A33:A61"/>
+    <mergeCell ref="A63:A76"/>
+    <mergeCell ref="A78:A86"/>
+    <mergeCell ref="A88:A98"/>
+    <mergeCell ref="A100:A111"/>
+    <mergeCell ref="A113:A123"/>
+    <mergeCell ref="A130:A165"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A166:A182"/>
     <mergeCell ref="A183:A191"/>
@@ -2833,17 +2857,6 @@
     <mergeCell ref="B163:C163"/>
     <mergeCell ref="B112:C112"/>
     <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="A6:A31"/>
-    <mergeCell ref="A33:A61"/>
-    <mergeCell ref="A63:A76"/>
-    <mergeCell ref="A78:A86"/>
-    <mergeCell ref="A88:A98"/>
-    <mergeCell ref="A100:A111"/>
-    <mergeCell ref="A113:A123"/>
-    <mergeCell ref="A130:A165"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2854,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88A73F7-8A1C-4AAA-956E-66E3E33E6302}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,229 +2883,229 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="F3" s="51"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="51"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>268</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="B2" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>279</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>266</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>275</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>283</v>
-      </c>
-      <c r="F3" s="50"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>277</v>
-      </c>
-      <c r="F4" s="50"/>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>274</v>
-      </c>
-      <c r="F5" s="51"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B6" s="18">
         <v>0.5</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="41"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>281</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="52">
-        <v>0.5</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="53" t="s">
-        <v>286</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>291</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="39" t="s">
+      <c r="E12" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="39"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="39" t="s">
-        <v>287</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>293</v>
-      </c>
-      <c r="F9" s="39"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="39" t="s">
-        <v>288</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="F10" s="39"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>295</v>
-      </c>
-      <c r="F11" s="39"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="39" t="s">
-        <v>289</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>297</v>
-      </c>
-      <c r="F12" s="39"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="42"/>
-      <c r="B13" s="43"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="42"/>
-      <c r="D13" s="39" t="s">
-        <v>290</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>296</v>
-      </c>
-      <c r="F13" s="39"/>
+      <c r="D13" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
-        <v>298</v>
-      </c>
-      <c r="B14" s="52">
+        <v>293</v>
+      </c>
+      <c r="B14" s="26">
         <v>1</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>280</v>
-      </c>
-      <c r="D14" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="47" t="s">
-        <v>300</v>
-      </c>
-      <c r="F14" s="47"/>
+      <c r="E14" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="47" t="s">
-        <v>299</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>301</v>
-      </c>
-      <c r="F15" s="47"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>20</v>
@@ -3144,15 +3157,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="C2:C5"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="C2:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3161,175 +3174,246 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D09C8A4-D8D1-40D7-A41A-731B28E4BBEE}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>239</v>
+        <v>299</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>241</v>
+        <v>300</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>243</v>
+        <v>307</v>
       </c>
       <c r="B15" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B16" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>244</v>
+        <v>302</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>254</v>
+        <v>303</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="C19" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20" s="54">
         <v>1</v>
       </c>
+      <c r="C20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B21" s="1">
+        <f>SUM(B2:B20)</f>
+        <v>22.5</v>
+      </c>
+      <c r="C21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3353,7 +3437,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="52" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3364,7 +3448,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
+      <c r="A2" s="52"/>
       <c r="B2" s="1" t="s">
         <v>141</v>
       </c>
@@ -3409,7 +3493,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="52" t="s">
         <v>162</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -3420,7 +3504,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="1" t="s">
         <v>152</v>
       </c>
@@ -3429,7 +3513,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="53" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -3440,7 +3524,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="1" t="s">
         <v>237</v>
       </c>
@@ -3449,7 +3533,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
@@ -3541,22 +3625,22 @@
       <c r="A18" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>256</v>
+      <c r="B18" s="19" t="s">
+        <v>251</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
-      <c r="B19" s="33" t="s">
-        <v>257</v>
+      <c r="B19" s="19" t="s">
+        <v>252</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
-      <c r="B20" s="33" t="s">
-        <v>258</v>
+      <c r="B20" s="19" t="s">
+        <v>253</v>
       </c>
       <c r="C20" s="1"/>
     </row>

</xml_diff>